<commit_message>
S03P23D105-10 | updated scripts
</commit_message>
<xml_diff>
--- a/back/fixtures/temp/scripts.xlsx
+++ b/back/fixtures/temp/scripts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\csvToExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="5688"/>
   </bookViews>
   <sheets>
     <sheet name="scripts" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>그 바람에 높은 호랑이 탑이 와르르 무너져 버렸어요</t>
   </si>
   <si>
-    <t>잠깐! 피리로 소리를 내어 호랑이 들을 겁먹게 해야겠어</t>
-  </si>
-  <si>
     <t>도시로 갔더니 한참 오디션이 진행중에 있었어요</t>
   </si>
   <si>
@@ -152,12 +149,6 @@
     <t>토끼랑 한참을 걷고 나니&lt;br&gt;다과회가 열리는 곳에 도착했어요</t>
   </si>
   <si>
-    <t>다과회에 참여하려면&lt;br&gt;귀중한 물품을 보여줘야되!&lt;br&gt;보여줄래?</t>
-  </si>
-  <si>
-    <t>곰곰히 생각한뒤&lt;br&gt;두 번째 선물로 받은 궤짝을 선물로 주기로 했어요</t>
-  </si>
-  <si>
     <t>오호! 처음보는 물품이야&lt;br&gt;너는 우리 다과회에 참여할 수 있겠어</t>
   </si>
   <si>
@@ -167,12 +158,6 @@
     <t>한 쪽에는 큰 나무가 보였고&lt;br&gt;한 쪽은 큰 빌딩이 보였어요</t>
   </si>
   <si>
-    <t>내가 3번쨰 선물로 받은&lt;br&gt;피리를 멋지게 불어야겠어</t>
-  </si>
-  <si>
-    <t>마을사람들이 쥐들을 없애려고 애를 썻지만&lt;br&gt;쥐들은 없어지지 않았어요</t>
-  </si>
-  <si>
     <t>그런데 쥐들이 피리소리를 들으니&lt;br&gt;놀라운 일이 일어났어요</t>
   </si>
   <si>
@@ -197,140 +182,161 @@
     <t>호랑이들이 기타소리에 흥이 나서&lt;br&gt;어깨를 들썩들썩, 궁둥이를 움찍움찔\춤을 추기 시작했어요</t>
   </si>
   <si>
+    <t>못된 호랑이들을 쫓아 주셔서 감사합니다.&lt;br&gt;모두 만세</t>
+  </si>
+  <si>
+    <t>너무 훌륭한 솜씨군!&lt;br&gt;나랑 함께 최고의 가수가 되지 않겠나?</t>
+  </si>
+  <si>
+    <t>아버지에게 3가지 선물을 받은 {child_name}(이)는&lt;br&gt;여행을 떠나기 시작했어요.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>담장 안을 빠끔 넘어다 보니&lt;br&gt;할머니가 곱게 단장한 신부에게 다가가고 있었어요.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>갑자기! 사람들 몰래 옆구리를 할퀴었어요.&lt;br&gt;그러자 말짱했던 신부가 풀썩 쓰러졌어요.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>여우는 할머니 모습으로 산을 내려갔어요.&lt;br&gt;그리고 혼례가 열리는 잔칫집으로 쏙 들어갔어요!</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{child_name}(이)는 첫번째 선물으로 여우를 혼내줬어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>토끼는 나무둥지 앞에 멈춰섰어요&lt;br&gt;그런데! 갑자기 토끼의 크기가 개미같이 줄어들었어요&lt;br&gt;그리고 나무구멍으로 들어갔어요.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>토끼는 어디로 가는거지?</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>여기숨어</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>도와줘~</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>나쁜 하트여왕!&lt;br&gt;토끼를 괴롭히지마</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>고마워~&lt;br&gt;나랑 놀러가지 않을래?</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>흑흑흑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>거기에는 청진기가 들어있었어요.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>너무 감사합니다&lt;br&gt;덕분에 확실히 나았어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{child_name}(이)는 첫번째 선물인 지팡이로&lt;br&gt;여왕을 물리쳤어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>그런데 갑자기, 나쁜 하트여왕이 나타나&lt;br&gt;토끼를 공격하기 시작했어요!</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>곧 험상궃은 독수리들이 다가왔어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>자느라 아무것도 못 봤어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>이렇게 쥐들을 무사히 쫓아 내었어요&lt;br&gt;그리고 마을에는 평화가 찾아왔답니다.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떻게 지나가지…&lt;br&gt;아 맞다! 피리로 곰을 깨워볼까?</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{child_name}(은)는 피리를 불기 시작했어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>재빠르게 나무 위로 올라갔지만&lt;br&gt;호랑이들도 하나 둘씩 올라오기 시작했어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>마지막 선물을 꺼내봐야겠어</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>바보 같은 호랑이들&lt;br&gt;피리 소리에 깜짝 놀라서 도망갔구나</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{child_name}(이)는 3번째 선물로 받은 기타로 놀라운 솜씨를 뽐내었어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>혹시 다람쥐를 보지 못했니?</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>그럼 다녀오너라&lt;br&gt;잘 갔다 오라는 의미로 3가지 선물을 주마</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>얼마 정도 갔을까&lt;br&gt;길의 한쪽에는 수상하게 웃고있는 여우가&lt;br&gt;다른 한쪽에는 다급해보이는 토끼가 있는걸 발견했어요.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>저 여우는 무슨 꿍꿍이 일까?&lt;br&gt;무슨일이 일어날 것만 같아</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무 앞으로 다가가니 {child_name}(이)의 몸이 개미같이 줄어들었어요!&lt;br&gt;그리고 나무 구멍을 통과한 토끼를 발견할 수 있었어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>다과회에 참여하려면&lt;br&gt;귀중한 물품을 보여줘야돼!&lt;br&gt;보여줄래?</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>곰곰이 생각한뒤&lt;br&gt;두 번째 선물로 받은 궤짝을 선물로 주기로 했어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 3번째 선물로 받은&lt;br&gt;피리를 멋지게 불어야겠어</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>그때, 음식 냄새를 맡은&lt;br&gt;크고 끔찍한 쥐들이 나타났어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>마을사람들이 쥐들을 없애려고 애를 썼지만&lt;br&gt;쥐들은 도망가지 않았어요</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠깐! 피리로 소리를 내어 호랑이들을 겁먹게 해야겠어</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>호랑이들은 철퍼덕 철퍼덕 떨어져&lt;br&gt;모두 죽고 말았어요</t>
-  </si>
-  <si>
-    <t>못된 호랑이들을 쫓아 주셔서 감사합니다.&lt;br&gt;모두 만세</t>
-  </si>
-  <si>
-    <t>너무 훌륭한 솜씨군!&lt;br&gt;나랑 함께 최고의 가수가 되지 않겠나?</t>
-  </si>
-  <si>
-    <t>그럼 다녀오너라&lt;br&gt;잘 갔다 와라는 의미로 3가지 선물을 주마</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>아버지에게 3가지 선물을 받은 {child_name}(이)는&lt;br&gt;여행을 떠나기 시작했어요.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>담장 안을 빠끔 넘어다 보니&lt;br&gt;할머니가 곱게 단장한 신부에게 다가가고 있었어요.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>갑자기! 사람들 몰래 옆구리를 할퀴었어요.&lt;br&gt;그러자 말짱했던 신부가 풀썩 쓰러졌어요.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>여우는 할머니 모습으로 산을 내려갔어요.&lt;br&gt;그리고 혼례가 열리는 잔칫집으로 쏙 들어갔어요!</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>얼마 정도 갔을까&lt;br&gt;길의 한쪽에는 수상하게 웃고있는 여우가&lt;br&gt;다른 한쪽에는 급해보이는 토끼가 있는걸 발견했어요.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>저 여우는 무슨 꿍꿍이 일까?&lt;br&gt;무슨일을 일어날 것만 같아</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>{child_name}(이)는 첫번째 선물으로 여우를 혼내줬어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>토끼는 나무둥지 앞에 멈춰섰어요&lt;br&gt;그런데! 갑자기 토끼의 크기가 개미같이 줄어들었어요&lt;br&gt;그리고 나무구멍으로 들어갔어요.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>토끼는 어디로 가는거지?</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>나무 앞에 섰더니 {child_name}(이)의 몸이 개미같이 줄어들었어요!&lt;br&gt;나무구멍을 통과하니 토끼를 발견할 수 있었어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>여기숨어</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>도와줘~</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>나쁜 하트여왕!&lt;br&gt;토끼를 괴롭히지마</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>고마워~&lt;br&gt;나랑 놀러가지 않을래?</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>흑흑흑</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>거기에는 청진기가 들어있었어요.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>너무 감사합니다&lt;br&gt;덕분에 확실히 나았어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>{child_name}(이)는 첫번째 선물인 지팡이로&lt;br&gt;여왕을 물리쳤어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>그런데 갑자기, 나쁜 하트여왕이 나타나&lt;br&gt;토끼를 공격하기 시작했어요!</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>곧 험상궃은 독수리들이 다가왔어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>자느라 아무것도 못 봤어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>그때, 음식을 냄새를 맡은&lt;br&gt;크고 끔찍한 쥐들이 나타났어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>이렇게 쥐들을 무사히 쫓아 내었어요&lt;br&gt;그리고 마을에는 평화가 찾아왔답니다.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>어떻게 지나가지…&lt;br&gt;아 맞다! 피리로 곰을 깨워볼까?</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>{child_name}(은)는 피리를 불기 시작했어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>재빠르게 나무 위로 올라갔지만&lt;br&gt;호랑이들도 하나 둘씩 올라오기 시작했어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>마지막 선물을 꺼내봐야겠어</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>바보 같은 호랑이들&lt;br&gt;피리 소리에 깜짝 놀라서 도망갔구나</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>피리를 불어 천둥같이 큰 소리를 냈어요&lt;br&gt;호랑이들은 꽁지 빠지게 도망갔어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>{child_name}(이)는 3번째 선물로 받은 기타로 놀라운 솜씨를 뽐내었어요</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>혹시 다람쥐를 보지 못했니?</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>피리를 불어 천둥같이 큰 소리를 냈어요&lt;br&gt;호랑이들은 철퍼덕 철퍼덕 떨어졌어요</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -338,7 +344,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -498,6 +504,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -924,8 +939,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1249,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="95" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1260,7 +1278,7 @@
     <col min="4" max="4" width="48.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1277,7 +1295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1288,13 +1306,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1305,13 +1323,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1322,13 +1340,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1339,13 +1357,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1356,13 +1374,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1373,13 +1391,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1390,13 +1408,13 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1407,13 +1425,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1424,13 +1442,14 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1444,10 +1463,11 @@
         <v>5</v>
       </c>
       <c r="E11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1461,10 +1481,11 @@
         <v>6</v>
       </c>
       <c r="E12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1475,13 +1496,14 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1492,13 +1514,14 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1509,13 +1532,14 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1526,13 +1550,14 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1543,13 +1568,14 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="E17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1560,13 +1586,14 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+        <v>10</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1577,13 +1604,14 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+        <v>10</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1594,13 +1622,14 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1611,13 +1640,14 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1628,13 +1658,14 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1645,13 +1676,14 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1662,13 +1694,14 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+        <v>13</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1679,13 +1712,14 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E25">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+        <v>13</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1696,13 +1730,14 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1713,13 +1748,14 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1730,13 +1766,14 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E28">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1747,13 +1784,14 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E29">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1764,13 +1802,14 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E30">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1784,10 +1823,11 @@
         <v>7</v>
       </c>
       <c r="E31">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1798,13 +1838,14 @@
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1815,13 +1856,14 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E33">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1832,13 +1874,14 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E34">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1849,13 +1892,14 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E35">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1866,13 +1910,14 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E36">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1883,13 +1928,14 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E37">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1903,10 +1949,11 @@
         <v>8</v>
       </c>
       <c r="E38">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1920,10 +1967,11 @@
         <v>9</v>
       </c>
       <c r="E39">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1937,10 +1985,11 @@
         <v>10</v>
       </c>
       <c r="E40">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1951,13 +2000,14 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E41">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1968,13 +2018,14 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E42">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1985,13 +2036,14 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="E43">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2002,13 +2054,14 @@
         <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="E44">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2019,13 +2072,14 @@
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E45">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2039,10 +2093,11 @@
         <v>11</v>
       </c>
       <c r="E46">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2056,10 +2111,11 @@
         <v>12</v>
       </c>
       <c r="E47">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2070,13 +2126,14 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E48">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2087,13 +2144,14 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E49">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2107,10 +2165,11 @@
         <v>13</v>
       </c>
       <c r="E50">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2121,13 +2180,14 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="E51">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2138,13 +2198,14 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E52">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+        <v>24</v>
+      </c>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2155,13 +2216,14 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="E53">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+        <v>24</v>
+      </c>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2172,13 +2234,14 @@
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E54">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+        <v>25</v>
+      </c>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2192,10 +2255,11 @@
         <v>14</v>
       </c>
       <c r="E55">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+        <v>25</v>
+      </c>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2209,10 +2273,11 @@
         <v>15</v>
       </c>
       <c r="E56">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+        <v>25</v>
+      </c>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2223,13 +2288,14 @@
         <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E57">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+        <v>25</v>
+      </c>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2243,10 +2309,11 @@
         <v>16</v>
       </c>
       <c r="E58">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2260,10 +2327,11 @@
         <v>17</v>
       </c>
       <c r="E59">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2274,13 +2342,14 @@
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E60">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2291,13 +2360,14 @@
         <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="E61">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2308,13 +2378,14 @@
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E62">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+        <v>27</v>
+      </c>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2325,13 +2396,14 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E63">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+        <v>27</v>
+      </c>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2342,13 +2414,14 @@
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E64">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+        <v>28</v>
+      </c>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2362,10 +2435,11 @@
         <v>18</v>
       </c>
       <c r="E65">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>64</v>
       </c>
@@ -2379,10 +2453,11 @@
         <v>19</v>
       </c>
       <c r="E66">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2393,13 +2468,14 @@
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E67">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2410,13 +2486,14 @@
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E68">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+        <v>32</v>
+      </c>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2427,13 +2504,14 @@
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E69">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>68</v>
       </c>
@@ -2444,13 +2522,14 @@
         <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E70">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>69</v>
       </c>
@@ -2461,13 +2540,14 @@
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E71">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>70</v>
       </c>
@@ -2478,13 +2558,14 @@
         <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E72">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>71</v>
       </c>
@@ -2498,10 +2579,11 @@
         <v>20</v>
       </c>
       <c r="E73">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>72</v>
       </c>
@@ -2512,13 +2594,14 @@
         <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="E74">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>73</v>
       </c>
@@ -2529,13 +2612,14 @@
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="E75">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>74</v>
       </c>
@@ -2546,13 +2630,14 @@
         <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E76">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>75</v>
       </c>
@@ -2563,13 +2648,14 @@
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E77">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+        <v>38</v>
+      </c>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>76</v>
       </c>
@@ -2580,13 +2666,14 @@
         <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E78">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>77</v>
       </c>
@@ -2597,13 +2684,14 @@
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E79">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
+        <v>40</v>
+      </c>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>78</v>
       </c>
@@ -2614,13 +2702,14 @@
         <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E80">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
+        <v>40</v>
+      </c>
+      <c r="G80" s="1"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>79</v>
       </c>
@@ -2631,13 +2720,14 @@
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E81">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>80</v>
       </c>
@@ -2648,13 +2738,14 @@
         <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E82">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>81</v>
       </c>
@@ -2665,13 +2756,14 @@
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E83">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>82</v>
       </c>
@@ -2682,13 +2774,14 @@
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E84">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>83</v>
       </c>
@@ -2699,13 +2792,14 @@
         <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E85">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>84</v>
       </c>
@@ -2716,13 +2810,14 @@
         <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E86">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
+        <v>45</v>
+      </c>
+      <c r="G86" s="1"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>85</v>
       </c>
@@ -2733,13 +2828,14 @@
         <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E87">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
+        <v>46</v>
+      </c>
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>86</v>
       </c>
@@ -2750,11 +2846,12 @@
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E88">
-        <v>41</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G88" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>